<commit_message>
Add placeholder values for lesson C
</commit_message>
<xml_diff>
--- a/data/tables/results.xlsx
+++ b/data/tables/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mag3842/GitHub/hunch/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F1D752-B737-7A44-87C6-5BD4F82B2039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAF59A7-F43E-9B4A-B9E7-89E3FBFF0EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>lesson</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Effective Temperature (K)</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EEE507-0F2C-5E46-BF79-43A8A96DBB8E}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,6 +784,138 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:E1"/>

</xml_diff>

<commit_message>
"update table with Lesson C results
</commit_message>
<xml_diff>
--- a/data/tables/results.xlsx
+++ b/data/tables/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mag3842/GitHub/hunch/data/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayicao/GitHub/puffyn/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAF59A7-F43E-9B4A-B9E7-89E3FBFF0EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C4FB70-4CF7-CD46-85DA-F8782C7B9C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
+    <workbookView xWindow="10000" yWindow="500" windowWidth="19360" windowHeight="16200" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
   </bookViews>
   <sheets>
     <sheet name="01_sonora_bobcat_2018" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,40 +528,40 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>-26.3</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -572,40 +572,40 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>31.15</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -616,40 +616,40 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>-7.35</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>20.55</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -660,22 +660,22 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -687,13 +687,13 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>-62.3</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>-23.8</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -704,22 +704,22 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -731,13 +731,13 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -748,22 +748,22 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -772,16 +772,16 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>-19.649999999999999</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -792,40 +792,40 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1675</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>-3.25</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>17.350000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -836,40 +836,40 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>32.1</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>46.85</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -880,40 +880,40 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>-38.549999999999997</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>-23</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>-15.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results table with complete answers for Lessons A through C
</commit_message>
<xml_diff>
--- a/data/tables/results.xlsx
+++ b/data/tables/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayicao/GitHub/puffyn/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C4FB70-4CF7-CD46-85DA-F8782C7B9C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E394140-AFC1-3D4E-8B3D-D70B989666EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="500" windowWidth="19360" windowHeight="16200" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
+    <workbookView xWindow="5100" yWindow="500" windowWidth="23100" windowHeight="16060" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
   </bookViews>
   <sheets>
     <sheet name="01_sonora_bobcat_2018" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,7 +531,7 @@
         <v>1700</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="E3">
         <v>2200</v>
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="H3">
         <v>4.75</v>
@@ -549,7 +549,7 @@
         <v>28.5</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>36.6</v>
       </c>
       <c r="K3">
         <v>40</v>
@@ -558,7 +558,7 @@
         <v>-26.3</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>-14</v>
       </c>
       <c r="N3">
         <v>0.75</v>
@@ -575,7 +575,7 @@
         <v>850</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="E4">
         <v>1300</v>
@@ -584,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>4.75</v>
@@ -593,7 +593,7 @@
         <v>16</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>21.3</v>
       </c>
       <c r="K4">
         <v>27</v>
@@ -602,7 +602,7 @@
         <v>31.15</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>41.8</v>
       </c>
       <c r="N4">
         <v>55.75</v>
@@ -619,7 +619,7 @@
         <v>650</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="E5">
         <v>1200</v>
@@ -628,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="H5">
         <v>5.5</v>
@@ -637,7 +637,7 @@
         <v>0.1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K5">
         <v>12.5</v>
@@ -646,7 +646,7 @@
         <v>-7.35</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>6.6</v>
       </c>
       <c r="N5">
         <v>20.55</v>
@@ -663,34 +663,34 @@
         <v>500</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E6">
         <v>800</v>
       </c>
       <c r="F6">
+        <v>4.5</v>
+      </c>
+      <c r="G6">
+        <v>4.75</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>5.25</v>
-      </c>
       <c r="I6">
-        <v>0</v>
+        <v>25.3</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L6">
         <v>-62.3</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>-41.75</v>
       </c>
       <c r="N6">
         <v>-23.8</v>
@@ -707,7 +707,7 @@
         <v>1900</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="E7">
         <v>2400</v>
@@ -716,28 +716,28 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="H7">
         <v>5.5</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L7">
         <v>0.8</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="N7">
-        <v>5.5</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>1600</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E8">
         <v>2100</v>
@@ -760,28 +760,28 @@
         <v>4</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="H8">
         <v>4.5</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>26.3</v>
       </c>
       <c r="K8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L8">
         <v>-19.649999999999999</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>-4.95</v>
       </c>
       <c r="N8">
-        <v>3.75</v>
+        <v>6.55</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
corrected table and updated jupyter notebook
</commit_message>
<xml_diff>
--- a/data/tables/results.xlsx
+++ b/data/tables/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayicao/GitHub/puffyn/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E394140-AFC1-3D4E-8B3D-D70B989666EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA3FFE0-AEBC-6742-9C88-71D65AB6CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="500" windowWidth="23100" windowHeight="16060" xr2:uid="{EDD55AC9-22B1-434D-BF90-70BD56650621}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +751,7 @@
         <v>1600</v>
       </c>
       <c r="D8">
-        <v>800</v>
+        <v>1800</v>
       </c>
       <c r="E8">
         <v>2100</v>

</xml_diff>